<commit_message>
Project Test Automation #2
</commit_message>
<xml_diff>
--- a/ReadData.xlsx
+++ b/ReadData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57170294512435a7/Desktop/UPES Content/Semester 6/Test Automation/EndSem Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse\Eclipse_Workspace_Java\TestAutomation.Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="278" documentId="11_946C2C743AF093F479D9A576D68EB0A46A50217A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F79010A7-E561-4787-8153-058C5F37C0E2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C808FCD-D720-4E34-BEA6-BE63A55FFD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,22 +32,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Password</t>
   </si>
   <si>
     <t>mayank_is_me</t>
+  </si>
+  <si>
+    <t>me_is_mayank</t>
+  </si>
+  <si>
+    <t>Email/Username</t>
+  </si>
+  <si>
+    <t>DevOps_TA</t>
+  </si>
+  <si>
+    <t>TA_DevOps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -59,6 +68,21 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -87,10 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -306,32 +332,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E8CB17-EC3E-4A77-A95D-8769C410B7F2}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>